<commit_message>
Remove mine project from this branch
</commit_message>
<xml_diff>
--- a/logic/lab3/kb.xlsx
+++ b/logic/lab3/kb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\ISC\Lenguajes\logic\lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\ISC\Lenguajes\programming_languages\logic\lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298FB65D-7CA9-46D4-90C5-E3E618C66907}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DBB506-6A15-4C2D-B245-1661C8B7CBEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6C8CF9D9-F323-48B3-9241-4ECFCAC3CD21}"/>
+    <workbookView xWindow="-28920" yWindow="-5985" windowWidth="29040" windowHeight="15840" xr2:uid="{6C8CF9D9-F323-48B3-9241-4ECFCAC3CD21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>mov(</t>
   </si>
@@ -46,12 +48,6 @@
   </si>
   <si>
     <t>Salidas</t>
-  </si>
-  <si>
-    <t>Niveles de alarma</t>
-  </si>
-  <si>
-    <t>Distancia que puedes recorrer</t>
   </si>
   <si>
     <t>mov(14,13).</t>
@@ -189,12 +185,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75AF719-B2E0-4891-A9AB-74AB83C3ADCE}">
-  <dimension ref="B3:AA37"/>
+  <dimension ref="B3:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,25 +972,25 @@
         <v>mov(95,96).</v>
       </c>
       <c r="U13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="V13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="W13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Y13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Z13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AA13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.25">
@@ -1028,22 +1022,22 @@
         <v>mov(96,97).</v>
       </c>
       <c r="V14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="W14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="X14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Z14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AA14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.25">
@@ -1072,19 +1066,19 @@
         <v>mov(72,73).</v>
       </c>
       <c r="V15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="W15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="X15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Y15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Z15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.25">
@@ -1097,7 +1091,7 @@
         <v>mov(66,67).</v>
       </c>
       <c r="Y16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
@@ -1110,7 +1104,7 @@
         <v>mov(67,68).</v>
       </c>
       <c r="Y17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
@@ -1119,402 +1113,362 @@
         <v>mov(68,69).</v>
       </c>
       <c r="Y18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2">
+        <v>6</v>
+      </c>
+      <c r="I22" s="4">
+        <v>7</v>
+      </c>
+      <c r="J22" s="4">
+        <v>8</v>
+      </c>
+      <c r="K22" s="4">
+        <v>9</v>
+      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2">
+        <v>11</v>
+      </c>
+      <c r="D23" s="4">
+        <v>12</v>
+      </c>
+      <c r="E23" s="2">
+        <v>13</v>
+      </c>
+      <c r="F23" s="2">
+        <v>14</v>
+      </c>
+      <c r="G23" s="4">
+        <v>15</v>
+      </c>
+      <c r="H23" s="2">
+        <v>16</v>
+      </c>
+      <c r="I23" s="4">
+        <v>17</v>
+      </c>
+      <c r="J23" s="4">
+        <v>18</v>
+      </c>
+      <c r="K23" s="4">
+        <v>19</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2">
+        <v>21</v>
+      </c>
+      <c r="D24" s="4">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="J19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="J20" s="4">
-        <v>1</v>
-      </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4">
-        <v>3</v>
-      </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="J21" s="4">
-        <v>2</v>
-      </c>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4">
-        <v>4</v>
-      </c>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="J22" s="4">
-        <v>3</v>
-      </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4">
-        <v>5</v>
-      </c>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="J23" s="4">
-        <v>4</v>
-      </c>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4">
-        <v>6</v>
-      </c>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
+      <c r="E24" s="2">
+        <v>23</v>
+      </c>
+      <c r="F24" s="4">
+        <v>24</v>
+      </c>
+      <c r="G24" s="4">
+        <v>25</v>
+      </c>
+      <c r="H24" s="2">
+        <v>26</v>
+      </c>
+      <c r="I24" s="2">
+        <v>27</v>
+      </c>
+      <c r="J24" s="2">
+        <v>28</v>
+      </c>
+      <c r="K24" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>30</v>
+      </c>
+      <c r="C25" s="2">
+        <v>31</v>
+      </c>
+      <c r="D25" s="2">
+        <v>32</v>
+      </c>
+      <c r="E25" s="2">
+        <v>33</v>
+      </c>
+      <c r="F25" s="4">
+        <v>34</v>
+      </c>
+      <c r="G25" s="2">
+        <v>35</v>
+      </c>
+      <c r="H25" s="2">
+        <v>36</v>
+      </c>
+      <c r="I25" s="4">
+        <v>37</v>
+      </c>
+      <c r="J25" s="4">
+        <v>38</v>
+      </c>
+      <c r="K25" s="4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>40</v>
+      </c>
+      <c r="C26" s="2">
+        <v>41</v>
+      </c>
+      <c r="D26" s="4">
+        <v>42</v>
+      </c>
+      <c r="E26" s="2">
+        <v>43</v>
+      </c>
+      <c r="F26" s="4">
+        <v>44</v>
+      </c>
+      <c r="G26" s="4">
+        <v>45</v>
+      </c>
+      <c r="H26" s="2">
+        <v>46</v>
+      </c>
+      <c r="I26" s="2">
+        <v>47</v>
+      </c>
+      <c r="J26" s="2">
+        <v>48</v>
+      </c>
+      <c r="K26" s="4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>50</v>
+      </c>
+      <c r="C27" s="4">
+        <v>51</v>
+      </c>
+      <c r="D27" s="4">
+        <v>52</v>
+      </c>
+      <c r="E27" s="2">
+        <v>53</v>
+      </c>
+      <c r="F27" s="4">
+        <v>54</v>
+      </c>
+      <c r="G27" s="4">
+        <v>55</v>
+      </c>
+      <c r="H27" s="4">
+        <v>56</v>
+      </c>
+      <c r="I27" s="4">
+        <v>57</v>
+      </c>
+      <c r="J27" s="2">
+        <v>58</v>
+      </c>
+      <c r="K27" s="4">
+        <v>59</v>
+      </c>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B28" s="5">
-        <v>0</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="5">
-        <v>2</v>
-      </c>
-      <c r="E28" s="5">
-        <v>3</v>
+      <c r="B28" s="4">
+        <v>60</v>
+      </c>
+      <c r="C28" s="4">
+        <v>61</v>
+      </c>
+      <c r="D28" s="4">
+        <v>62</v>
+      </c>
+      <c r="E28" s="2">
+        <v>63</v>
       </c>
       <c r="F28" s="2">
-        <v>4</v>
-      </c>
-      <c r="G28" s="5">
-        <v>5</v>
+        <v>64</v>
+      </c>
+      <c r="G28" s="2">
+        <v>65</v>
       </c>
       <c r="H28" s="2">
-        <v>6</v>
-      </c>
-      <c r="I28" s="5">
-        <v>7</v>
-      </c>
-      <c r="J28" s="5">
-        <v>8</v>
-      </c>
-      <c r="K28" s="5">
-        <v>9</v>
+        <v>66</v>
+      </c>
+      <c r="I28" s="2">
+        <v>67</v>
+      </c>
+      <c r="J28" s="2">
+        <v>68</v>
+      </c>
+      <c r="K28" s="2">
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B29" s="5">
-        <v>10</v>
+      <c r="B29" s="2">
+        <v>70</v>
       </c>
       <c r="C29" s="2">
-        <v>11</v>
-      </c>
-      <c r="D29" s="5">
-        <v>12</v>
+        <v>71</v>
+      </c>
+      <c r="D29" s="2">
+        <v>72</v>
       </c>
       <c r="E29" s="2">
-        <v>13</v>
-      </c>
-      <c r="F29" s="2">
-        <v>14</v>
-      </c>
-      <c r="G29" s="5">
-        <v>15</v>
-      </c>
-      <c r="H29" s="2">
-        <v>16</v>
-      </c>
-      <c r="I29" s="5">
-        <v>17</v>
-      </c>
-      <c r="J29" s="5">
-        <v>18</v>
-      </c>
-      <c r="K29" s="5">
-        <v>19</v>
+        <v>73</v>
+      </c>
+      <c r="F29" s="4">
+        <v>74</v>
+      </c>
+      <c r="G29" s="2">
+        <v>75</v>
+      </c>
+      <c r="H29" s="4">
+        <v>76</v>
+      </c>
+      <c r="I29" s="4">
+        <v>77</v>
+      </c>
+      <c r="J29" s="4">
+        <v>78</v>
+      </c>
+      <c r="K29" s="2">
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B30" s="5">
-        <v>20</v>
-      </c>
-      <c r="C30" s="2">
-        <v>21</v>
-      </c>
-      <c r="D30" s="5">
-        <v>22</v>
-      </c>
-      <c r="E30" s="2">
-        <v>23</v>
-      </c>
-      <c r="F30" s="5">
-        <v>24</v>
-      </c>
-      <c r="G30" s="5">
-        <v>25</v>
-      </c>
-      <c r="H30" s="2">
-        <v>26</v>
-      </c>
-      <c r="I30" s="2">
-        <v>27</v>
-      </c>
-      <c r="J30" s="2">
-        <v>28</v>
-      </c>
-      <c r="K30" s="2">
-        <v>29</v>
+      <c r="B30" s="4">
+        <v>80</v>
+      </c>
+      <c r="C30" s="4">
+        <v>81</v>
+      </c>
+      <c r="D30" s="4">
+        <v>82</v>
+      </c>
+      <c r="E30" s="4">
+        <v>83</v>
+      </c>
+      <c r="F30" s="4">
+        <v>84</v>
+      </c>
+      <c r="G30" s="2">
+        <v>85</v>
+      </c>
+      <c r="H30" s="4">
+        <v>86</v>
+      </c>
+      <c r="I30" s="4">
+        <v>87</v>
+      </c>
+      <c r="J30" s="4">
+        <v>88</v>
+      </c>
+      <c r="K30" s="4">
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B31" s="5">
-        <v>30</v>
-      </c>
-      <c r="C31" s="2">
-        <v>31</v>
-      </c>
-      <c r="D31" s="2">
-        <v>32</v>
-      </c>
-      <c r="E31" s="2">
-        <v>33</v>
-      </c>
-      <c r="F31" s="5">
-        <v>34</v>
+      <c r="B31" s="4">
+        <v>90</v>
+      </c>
+      <c r="C31" s="4">
+        <v>91</v>
+      </c>
+      <c r="D31" s="4">
+        <v>92</v>
+      </c>
+      <c r="E31" s="4">
+        <v>93</v>
+      </c>
+      <c r="F31" s="4">
+        <v>94</v>
       </c>
       <c r="G31" s="2">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="H31" s="2">
-        <v>36</v>
-      </c>
-      <c r="I31" s="5">
-        <v>37</v>
-      </c>
-      <c r="J31" s="5">
-        <v>38</v>
-      </c>
-      <c r="K31" s="5">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
-        <v>40</v>
-      </c>
-      <c r="C32" s="2">
-        <v>41</v>
-      </c>
-      <c r="D32" s="5">
-        <v>42</v>
-      </c>
-      <c r="E32" s="2">
-        <v>43</v>
-      </c>
-      <c r="F32" s="5">
-        <v>44</v>
-      </c>
-      <c r="G32" s="5">
-        <v>45</v>
-      </c>
-      <c r="H32" s="2">
-        <v>46</v>
-      </c>
-      <c r="I32" s="2">
-        <v>47</v>
-      </c>
-      <c r="J32" s="2">
-        <v>48</v>
-      </c>
-      <c r="K32" s="5">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="5">
-        <v>50</v>
-      </c>
-      <c r="C33" s="5">
-        <v>51</v>
-      </c>
-      <c r="D33" s="5">
-        <v>52</v>
-      </c>
-      <c r="E33" s="2">
-        <v>53</v>
-      </c>
-      <c r="F33" s="5">
-        <v>54</v>
-      </c>
-      <c r="G33" s="5">
-        <v>55</v>
-      </c>
-      <c r="H33" s="5">
-        <v>56</v>
-      </c>
-      <c r="I33" s="5">
-        <v>57</v>
-      </c>
-      <c r="J33" s="2">
-        <v>58</v>
-      </c>
-      <c r="K33" s="5">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="5">
-        <v>60</v>
-      </c>
-      <c r="C34" s="5">
-        <v>61</v>
-      </c>
-      <c r="D34" s="5">
-        <v>62</v>
-      </c>
-      <c r="E34" s="2">
-        <v>63</v>
-      </c>
-      <c r="F34" s="2">
-        <v>64</v>
-      </c>
-      <c r="G34" s="2">
-        <v>65</v>
-      </c>
-      <c r="H34" s="2">
-        <v>66</v>
-      </c>
-      <c r="I34" s="2">
-        <v>67</v>
-      </c>
-      <c r="J34" s="2">
-        <v>68</v>
-      </c>
-      <c r="K34" s="2">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
-        <v>70</v>
-      </c>
-      <c r="C35" s="2">
-        <v>71</v>
-      </c>
-      <c r="D35" s="2">
-        <v>72</v>
-      </c>
-      <c r="E35" s="2">
-        <v>73</v>
-      </c>
-      <c r="F35" s="5">
-        <v>74</v>
-      </c>
-      <c r="G35" s="2">
-        <v>75</v>
-      </c>
-      <c r="H35" s="5">
-        <v>76</v>
-      </c>
-      <c r="I35" s="5">
-        <v>77</v>
-      </c>
-      <c r="J35" s="5">
-        <v>78</v>
-      </c>
-      <c r="K35" s="2">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="5">
-        <v>80</v>
-      </c>
-      <c r="C36" s="5">
-        <v>81</v>
-      </c>
-      <c r="D36" s="5">
-        <v>82</v>
-      </c>
-      <c r="E36" s="5">
-        <v>83</v>
-      </c>
-      <c r="F36" s="5">
-        <v>84</v>
-      </c>
-      <c r="G36" s="2">
-        <v>85</v>
-      </c>
-      <c r="H36" s="5">
-        <v>86</v>
-      </c>
-      <c r="I36" s="5">
-        <v>87</v>
-      </c>
-      <c r="J36" s="5">
-        <v>88</v>
-      </c>
-      <c r="K36" s="5">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="5">
-        <v>90</v>
-      </c>
-      <c r="C37" s="5">
-        <v>91</v>
-      </c>
-      <c r="D37" s="5">
-        <v>92</v>
-      </c>
-      <c r="E37" s="5">
-        <v>93</v>
-      </c>
-      <c r="F37" s="5">
-        <v>94</v>
-      </c>
-      <c r="G37" s="2">
-        <v>95</v>
-      </c>
-      <c r="H37" s="2">
         <v>96</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I31" s="2">
         <v>97</v>
       </c>
-      <c r="J37" s="5">
+      <c r="J31" s="4">
         <v>98</v>
       </c>
-      <c r="K37" s="5">
+      <c r="K31" s="4">
         <v>99</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="J23:L23"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>